<commit_message>
updates to methods, definitions, parent project
</commit_message>
<xml_diff>
--- a/nes-lter-attune-fcm-discrete-transect-info.xlsx
+++ b/nes-lter-attune-fcm-discrete-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-attune-fcm-discrete-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA15A801-35F0-475D-9AB1-273DBBE5ABEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F76D93-4861-40A0-A65E-5013FFD002D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="182">
   <si>
     <t>keyword</t>
   </si>
@@ -551,12 +551,6 @@
     <t>indicates agreement: the cast and niskin in the filename matches a sample that was recorded as being taken</t>
   </si>
   <si>
-    <t>indicates missing data: a sample was supposedly taken, but no matching .fcs files were found</t>
-  </si>
-  <si>
-    <t>indicates questionable data: an .fcs file exists, but the sample log did not document that a sample was taken from the cast and niskin indicated by the filename. In some of these cases, we have manually identified which sample the .fcs data are most likely to correspond to: for example if the log indicates that an alternate niskin was used when that in the filename misfired. The filenames themselves are unchanged during this manual reassignment, so the adjustments are trackable by comparing the filenames to the cast and niskin columns</t>
-  </si>
-  <si>
     <t>indicates unevaluated: the .fcs filename has not yet been compared to the sample log</t>
   </si>
   <si>
@@ -567,6 +561,15 @@
   </si>
   <si>
     <t>Heterotrophic prokaryotes with relatively low nucleic acid</t>
+  </si>
+  <si>
+    <t>Distance greater than 2 km from NES-LTER station</t>
+  </si>
+  <si>
+    <t>indicates missing data: a sample was marked in the cruise sample log as collected, but no matching .fcs files were found</t>
+  </si>
+  <si>
+    <t>indicates questionable data: an .fcs file exists, but the sample log did not document that a sample was taken from the cast and niskin indicated by the filename. In some of these cases, we have manually identified which sample the .fcs data is most likely to correspond to.</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -647,15 +650,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -965,15 +964,16 @@
   </sheetPr>
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="207.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1110,45 +1110,45 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="7" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>163</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>87</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>88</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1816,7 +1816,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1843,7 +1843,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>174</v>
       </c>
     </row>
@@ -1854,8 +1854,8 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>175</v>
+      <c r="C3" s="6" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1865,8 +1865,8 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>176</v>
+      <c r="C4" s="6" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1876,8 +1876,8 @@
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>177</v>
+      <c r="C5" s="6" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2111,7 +2111,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>59</v>
       </c>
@@ -2151,7 +2151,7 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
station_distance and minor edits to Settings
</commit_message>
<xml_diff>
--- a/nes-lter-attune-fcm-discrete-transect-info.xlsx
+++ b/nes-lter-attune-fcm-discrete-transect-info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sosiknas1\Lab_data\Attune\EDI_data_packages\Attune_transect_FCMdiscrete\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-attune-fcm-discrete-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC86250-94DF-4048-A5B7-F9E85AAA4831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6475DC0B-6CBD-46C2-81B8-C9A59585E7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -515,9 +515,6 @@
     <t>nearest_station</t>
   </si>
   <si>
-    <t>distance_km</t>
-  </si>
-  <si>
     <t>abundance per milliliter of heterotrophic prokaryotic cells http://vocab.nerc.ac.uk/collection/F02/current/F0200010/ and http://vocab.nerc.ac.uk/collection/F02/current/F0200011/</t>
   </si>
   <si>
@@ -570,6 +567,9 @@
   </si>
   <si>
     <t>micrograms of carbon per liter of seawater of all measured eukaryote (urn:lsid:algaebase.org:taxname:86701) phytoplankton cells less than 20 um in diameter including cells counted in previous columns http://vocab.nerc.ac.uk/collection/F02/current/F0200004/ and http://vocab.nerc.ac.uk/collection/F02/current/F0200005/</t>
+  </si>
+  <si>
+    <t>station_distance</t>
   </si>
 </sst>
 </file>
@@ -964,19 +964,19 @@
   </sheetPr>
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="207.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="41.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="207.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -999,7 +999,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>83</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>89</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>91</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>94</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>96</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>99</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>100</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>102</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>106</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>109</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>111</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>113</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>116</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>119</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>121</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>122</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>124</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>126</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>127</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>129</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>131</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>132</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>134</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>136</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>137</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>139</v>
       </c>
@@ -1529,12 +1529,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="1" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>85</v>
@@ -1549,12 +1549,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>85</v>
@@ -1569,12 +1569,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>85</v>
@@ -1589,7 +1589,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>144</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>146</v>
       </c>
@@ -1626,12 +1626,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>85</v>
@@ -1646,12 +1646,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>85</v>
@@ -1666,7 +1666,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>149</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>151</v>
       </c>
@@ -1703,15 +1703,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>161</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>87</v>
@@ -1720,12 +1720,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>162</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>82</v>
@@ -1737,24 +1737,24 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1771,12 +1771,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -1820,12 +1820,12 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>161</v>
       </c>
@@ -1844,10 +1844,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -1855,10 +1855,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -1866,10 +1866,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1896,13 +1896,13 @@
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>59</v>
       </c>
@@ -2151,17 +2151,17 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2193,15 +2193,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2257,23 +2257,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>

</xml_diff>